<commit_message>
Month Merge & Unmerge Fix, Bug Fixes and File Update
</commit_message>
<xml_diff>
--- a/Excel/Mingguan/Excel/List Tugas Minggu Ke-5 (23 Agustus 2021 - 29 Agustus 2021).xlsx
+++ b/Excel/Mingguan/Excel/List Tugas Minggu Ke-5 (23 Agustus 2021 - 29 Agustus 2021).xlsx
@@ -697,8 +697,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I3" s="12" t="inlineStr"/>
-      <c r="J3" s="18" t="inlineStr"/>
+      <c r="I3" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J3" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="15.6" customHeight="1" s="1">
       <c r="A4" s="12" t="n">
@@ -781,8 +789,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I5" s="12" t="inlineStr"/>
-      <c r="J5" s="18" t="inlineStr"/>
+      <c r="I5" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J5" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="15.6" customHeight="1" s="1">
       <c r="A6" s="12" t="n">
@@ -799,7 +815,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E6" s="12" t="inlineStr"/>
+      <c r="E6" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="F6" s="17" t="inlineStr">
         <is>
           <t>ü</t>
@@ -816,7 +836,11 @@
         </is>
       </c>
       <c r="I6" s="12" t="inlineStr"/>
-      <c r="J6" s="18" t="inlineStr"/>
+      <c r="J6" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="15.6" customHeight="1" s="1">
       <c r="A7" s="12" t="n">
@@ -842,7 +866,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="F7" s="18" t="inlineStr"/>
+      <c r="F7" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="G7" s="16" t="inlineStr">
         <is>
           <t>ü</t>
@@ -853,8 +881,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I7" s="12" t="inlineStr"/>
-      <c r="J7" s="18" t="inlineStr"/>
+      <c r="I7" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J7" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="15.6" customHeight="1" s="1">
       <c r="A8" s="12" t="n">
@@ -933,8 +969,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I9" s="12" t="inlineStr"/>
-      <c r="J9" s="18" t="inlineStr"/>
+      <c r="I9" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J9" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="15.6" customHeight="1" s="1">
       <c r="A10" s="12" t="n">
@@ -1002,7 +1046,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="J11" s="18" t="inlineStr"/>
+      <c r="J11" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="15.6" customHeight="1" s="1">
       <c r="A12" s="12" t="n">
@@ -1019,7 +1067,11 @@
         </is>
       </c>
       <c r="D12" s="18" t="inlineStr"/>
-      <c r="E12" s="12" t="inlineStr"/>
+      <c r="E12" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="F12" s="18" t="inlineStr"/>
       <c r="G12" s="16" t="inlineStr">
         <is>
@@ -1049,8 +1101,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E13" s="12" t="inlineStr"/>
-      <c r="F13" s="18" t="inlineStr"/>
+      <c r="E13" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="F13" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="G13" s="16" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1061,8 +1121,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I13" s="12" t="inlineStr"/>
-      <c r="J13" s="18" t="inlineStr"/>
+      <c r="I13" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J13" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="15.6" customHeight="1" s="1">
       <c r="A14" s="12" t="n">
@@ -1103,8 +1171,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I14" s="12" t="inlineStr"/>
-      <c r="J14" s="18" t="inlineStr"/>
+      <c r="I14" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J14" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="15.6" customHeight="1" s="1">
       <c r="A15" s="12" t="n">
@@ -1125,7 +1201,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E15" s="12" t="inlineStr"/>
+      <c r="E15" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="F15" s="17" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1141,8 +1221,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I15" s="12" t="inlineStr"/>
-      <c r="J15" s="18" t="inlineStr"/>
+      <c r="I15" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J15" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="15.6" customHeight="1" s="1">
       <c r="A16" s="12" t="n">
@@ -1163,14 +1251,26 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E16" s="12" t="inlineStr"/>
-      <c r="F16" s="18" t="inlineStr"/>
+      <c r="E16" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="F16" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="G16" s="16" t="inlineStr">
         <is>
           <t>ü</t>
         </is>
       </c>
-      <c r="H16" s="18" t="inlineStr"/>
+      <c r="H16" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="I16" s="12" t="inlineStr"/>
       <c r="J16" s="18" t="inlineStr"/>
     </row>
@@ -1183,7 +1283,11 @@
           <t>Muhammad Asmaul Adam</t>
         </is>
       </c>
-      <c r="C17" s="12" t="inlineStr"/>
+      <c r="C17" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1195,8 +1299,16 @@
         </is>
       </c>
       <c r="F17" s="18" t="inlineStr"/>
-      <c r="G17" s="12" t="inlineStr"/>
-      <c r="H17" s="18" t="inlineStr"/>
+      <c r="G17" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="H17" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="I17" s="12" t="inlineStr"/>
       <c r="J17" s="18" t="inlineStr"/>
     </row>
@@ -1235,8 +1347,16 @@
         </is>
       </c>
       <c r="H18" s="18" t="inlineStr"/>
-      <c r="I18" s="12" t="inlineStr"/>
-      <c r="J18" s="18" t="inlineStr"/>
+      <c r="I18" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J18" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="15.6" customHeight="1" s="1">
       <c r="A19" s="12" t="n">
@@ -1247,7 +1367,11 @@
           <t>Muhammad Farhan</t>
         </is>
       </c>
-      <c r="C19" s="12" t="inlineStr"/>
+      <c r="C19" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="D19" s="17" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1258,7 +1382,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="F19" s="18" t="inlineStr"/>
+      <c r="F19" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="G19" s="16" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1269,8 +1397,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I19" s="12" t="inlineStr"/>
-      <c r="J19" s="18" t="inlineStr"/>
+      <c r="I19" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J19" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="15.6" customHeight="1" s="1">
       <c r="A20" s="12" t="n">
@@ -1291,7 +1427,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E20" s="12" t="inlineStr"/>
+      <c r="E20" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="F20" s="17" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1303,8 +1443,16 @@
         </is>
       </c>
       <c r="H20" s="18" t="inlineStr"/>
-      <c r="I20" s="12" t="inlineStr"/>
-      <c r="J20" s="18" t="inlineStr"/>
+      <c r="I20" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J20" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="15.6" customHeight="1" s="1">
       <c r="A21" s="12" t="n">
@@ -1325,16 +1473,28 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E21" s="12" t="inlineStr"/>
+      <c r="E21" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="F21" s="18" t="inlineStr"/>
       <c r="G21" s="16" t="inlineStr">
         <is>
           <t>ü</t>
         </is>
       </c>
-      <c r="H21" s="18" t="inlineStr"/>
+      <c r="H21" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="I21" s="12" t="inlineStr"/>
-      <c r="J21" s="18" t="inlineStr"/>
+      <c r="J21" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="15.6" customHeight="1" s="1">
       <c r="A22" s="12" t="n">
@@ -1351,7 +1511,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E22" s="12" t="inlineStr"/>
+      <c r="E22" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="F22" s="17" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1362,7 +1526,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="H22" s="18" t="inlineStr"/>
+      <c r="H22" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="I22" s="12" t="inlineStr"/>
       <c r="J22" s="18" t="inlineStr"/>
     </row>
@@ -1375,16 +1543,32 @@
           <t>Muhammad Yusuf</t>
         </is>
       </c>
-      <c r="C23" s="12" t="inlineStr"/>
+      <c r="C23" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="D23" s="18" t="inlineStr"/>
-      <c r="E23" s="12" t="inlineStr"/>
-      <c r="F23" s="18" t="inlineStr"/>
+      <c r="E23" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="F23" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="G23" s="16" t="inlineStr">
         <is>
           <t>ü</t>
         </is>
       </c>
-      <c r="H23" s="18" t="inlineStr"/>
+      <c r="H23" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="I23" s="12" t="inlineStr"/>
       <c r="J23" s="18" t="inlineStr"/>
     </row>
@@ -1412,7 +1596,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="F24" s="18" t="inlineStr"/>
+      <c r="F24" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="G24" s="16" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1423,8 +1611,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I24" s="12" t="inlineStr"/>
-      <c r="J24" s="18" t="inlineStr"/>
+      <c r="I24" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J24" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="25" ht="15.6" customHeight="1" s="1">
       <c r="A25" s="12" t="n">
@@ -1495,7 +1691,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E26" s="12" t="inlineStr"/>
+      <c r="E26" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="F26" s="17" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1511,8 +1711,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I26" s="12" t="inlineStr"/>
-      <c r="J26" s="18" t="inlineStr"/>
+      <c r="I26" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J26" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="15.6" customHeight="1" s="1">
       <c r="A27" s="12" t="n">
@@ -1523,7 +1731,11 @@
           <t>Nouridza Juniansah Ridhan</t>
         </is>
       </c>
-      <c r="C27" s="12" t="inlineStr"/>
+      <c r="C27" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="D27" s="17" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1534,7 +1746,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="F27" s="18" t="inlineStr"/>
+      <c r="F27" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="G27" s="16" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1546,7 +1762,11 @@
         </is>
       </c>
       <c r="I27" s="12" t="inlineStr"/>
-      <c r="J27" s="18" t="inlineStr"/>
+      <c r="J27" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="15.6" customHeight="1" s="1">
       <c r="A28" s="12" t="n">
@@ -1567,7 +1787,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E28" s="12" t="inlineStr"/>
+      <c r="E28" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="F28" s="17" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1588,7 +1812,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="J28" s="18" t="inlineStr"/>
+      <c r="J28" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="15.6" customHeight="1" s="1">
       <c r="A29" s="12" t="n">
@@ -1601,7 +1829,11 @@
       </c>
       <c r="C29" s="12" t="inlineStr"/>
       <c r="D29" s="18" t="inlineStr"/>
-      <c r="E29" s="12" t="inlineStr"/>
+      <c r="E29" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="F29" s="18" t="inlineStr"/>
       <c r="G29" s="16" t="inlineStr">
         <is>
@@ -1694,7 +1926,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="J31" s="18" t="inlineStr"/>
+      <c r="J31" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="32" ht="15.6" customHeight="1" s="1">
       <c r="A32" s="12" t="n">
@@ -1715,8 +1951,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E32" s="12" t="inlineStr"/>
-      <c r="F32" s="18" t="inlineStr"/>
+      <c r="E32" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="F32" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="G32" s="16" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1728,7 +1972,11 @@
         </is>
       </c>
       <c r="I32" s="12" t="inlineStr"/>
-      <c r="J32" s="18" t="inlineStr"/>
+      <c r="J32" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="33" ht="15.6" customHeight="1" s="1">
       <c r="A33" s="12" t="n">
@@ -1769,8 +2017,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I33" s="12" t="inlineStr"/>
-      <c r="J33" s="18" t="inlineStr"/>
+      <c r="I33" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="J33" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="34" ht="15.6" customHeight="1" s="1">
       <c r="A34" s="12" t="n">
@@ -1791,8 +2047,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E34" s="12" t="inlineStr"/>
-      <c r="F34" s="18" t="inlineStr"/>
+      <c r="E34" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="F34" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="G34" s="16" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1829,7 +2093,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E35" s="12" t="inlineStr"/>
+      <c r="E35" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="F35" s="17" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1875,15 +2143,31 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E36" s="12" t="inlineStr"/>
-      <c r="F36" s="18" t="inlineStr"/>
+      <c r="E36" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="F36" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="G36" s="16" t="inlineStr">
         <is>
           <t>ü</t>
         </is>
       </c>
-      <c r="H36" s="18" t="inlineStr"/>
-      <c r="I36" s="12" t="inlineStr"/>
+      <c r="H36" s="17" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="I36" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="J36" s="18" t="inlineStr"/>
     </row>
     <row r="37" ht="15.6" customHeight="1" s="1">
@@ -1905,7 +2189,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="E37" s="12" t="inlineStr"/>
+      <c r="E37" s="16" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="F37" s="17" t="inlineStr">
         <is>
           <t>ü</t>

</xml_diff>